<commit_message>
ECP-1303: splits removal of activities and sectors in SectorAndActivityImportManager
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/sector_and_activity_import_correct.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/sector_and_activity_import_correct.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Activity Description</t>
   </si>
@@ -31,10 +31,10 @@
     <t>Sector Sort Order</t>
   </si>
   <si>
-    <t>FASHION</t>
+    <t>ALL</t>
   </si>
   <si>
-    <t>ALL</t>
+    <t>FASHION</t>
   </si>
   <si>
     <t>ELECTRIC</t>
@@ -43,10 +43,10 @@
     <t>Test</t>
   </si>
   <si>
-    <t>TEST1</t>
+    <t>TEST</t>
   </si>
   <si>
-    <t>TEST</t>
+    <t>TEST1</t>
   </si>
   <si>
     <t>TEST2</t>
@@ -66,10 +66,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -85,27 +82,64 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -327,21 +361,22 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="4"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -363,17 +398,21 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -395,21 +434,21 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
+      <c r="A3" s="5" t="s">
+        <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
+      <c r="C3" s="2"/>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
+      <c r="E3" s="5" t="s">
+        <v>8</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -431,17 +470,21 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -463,21 +506,17 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -499,17 +538,13 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -531,21 +566,13 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -567,17 +594,13 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -599,13 +622,13 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -627,13 +650,13 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -655,13 +678,13 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -683,13 +706,13 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -711,13 +734,13 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -739,13 +762,13 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -28346,6 +28369,34 @@
       <c r="Y999" s="1"/>
       <c r="Z999" s="1"/>
     </row>
+    <row r="1000">
+      <c r="A1000" s="1"/>
+      <c r="B1000" s="1"/>
+      <c r="C1000" s="1"/>
+      <c r="D1000" s="1"/>
+      <c r="E1000" s="1"/>
+      <c r="F1000" s="1"/>
+      <c r="G1000" s="1"/>
+      <c r="H1000" s="1"/>
+      <c r="I1000" s="1"/>
+      <c r="J1000" s="1"/>
+      <c r="K1000" s="1"/>
+      <c r="L1000" s="1"/>
+      <c r="M1000" s="1"/>
+      <c r="N1000" s="1"/>
+      <c r="O1000" s="1"/>
+      <c r="P1000" s="1"/>
+      <c r="Q1000" s="1"/>
+      <c r="R1000" s="1"/>
+      <c r="S1000" s="1"/>
+      <c r="T1000" s="1"/>
+      <c r="U1000" s="1"/>
+      <c r="V1000" s="1"/>
+      <c r="W1000" s="1"/>
+      <c r="X1000" s="1"/>
+      <c r="Y1000" s="1"/>
+      <c r="Z1000" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>

</xml_diff>